<commit_message>
created by columns + project migrations
</commit_message>
<xml_diff>
--- a/public/uploads/Template contact.xlsx
+++ b/public/uploads/Template contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bemax/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59FBAF-4E4A-AD44-B7F7-23FE8A4C2558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0278E23-C810-0E49-9084-D43106D5F764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,7 +809,7 @@
   <dimension ref="A2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>